<commit_message>
Them word va powerpoint
</commit_message>
<xml_diff>
--- a/Documents/CNPM.xlsx
+++ b/Documents/CNPM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NhapSanPham" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>ID loại sản phẩm</t>
   </si>
@@ -406,92 +406,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="120.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="60.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1300000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1300000</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E3" s="1">
+        <v>1000000</v>
+      </c>
       <c r="F3" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="G3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -667,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>